<commit_message>
47 BRAND FIX SUM
</commit_message>
<xml_diff>
--- a/Excel/47 Brand/26.05.2022 47 BRAND — загрузка.xlsx
+++ b/Excel/47 Brand/26.05.2022 47 BRAND — загрузка.xlsx
@@ -3,9 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{29C1D22F-6C76-49A0-B2F6-BB0AC1C95149}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BUH\Documents\HatsAndCaps\Excel\47 Brand\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{060F2A8A-590E-4C9C-9F59-AA097E5F7FE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{EDC0FDC1-B8ED-46C2-BE83-FF1FAE39E9A4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7AD713A7-FE3C-4508-A782-EA575B3CF296}"/>
   </bookViews>
   <sheets>
     <sheet name="Загрузка" sheetId="1" r:id="rId1"/>
@@ -41,7 +46,7 @@
     <author>general</author>
   </authors>
   <commentList>
-    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{498184E3-7953-481E-9632-12BE3C487796}">
+    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{7E4E0275-CDC3-4693-8033-9B186D7DB3E6}">
       <text>
         <r>
           <rPr>
@@ -2688,8 +2693,8 @@
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
-    <cellStyle name="Обычный 8" xfId="1" xr:uid="{E6612B2F-407B-41E0-8208-5BFCF868C1B6}"/>
-    <cellStyle name="Финансовый 3" xfId="2" xr:uid="{CA2EDF5F-8BAD-49DE-A4B4-E18F136C6589}"/>
+    <cellStyle name="Обычный 8" xfId="1" xr:uid="{A6850AE7-6B36-495A-BA82-3E9C7B5545D3}"/>
+    <cellStyle name="Финансовый 3" xfId="2" xr:uid="{80D48FA4-B242-4056-87F4-BAA2ED2AF8F1}"/>
   </cellStyles>
   <dxfs count="1">
     <dxf>
@@ -2714,7 +2719,6 @@
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
-      <sheetName val="Загрузка"/>
       <sheetName val="Товары"/>
       <sheetName val="Форма"/>
       <sheetName val="Размеры"/>
@@ -2754,8 +2758,7 @@
       <sheetData sheetId="15"/>
       <sheetData sheetId="16"/>
       <sheetData sheetId="17"/>
-      <sheetData sheetId="18"/>
-      <sheetData sheetId="19">
+      <sheetData sheetId="18">
         <row r="2">
           <cell r="C2" t="str">
             <v>Строчный!S1:S135</v>
@@ -3063,15 +3066,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E054F0A5-AC16-4857-836F-7370E64303D3}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC1EFD44-7850-462D-85EB-7F6D45547368}">
   <sheetPr codeName="Лист28">
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
   <dimension ref="A1:Y135"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AT1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A110" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AT3" sqref="AT3"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="R1" sqref="R1:R1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3227,7 +3230,7 @@
       </c>
       <c r="P2"/>
       <c r="Q2">
-        <v>1651.65</v>
+        <v>1551.55</v>
       </c>
       <c r="R2" t="s">
         <v>39</v>
@@ -3300,7 +3303,7 @@
       </c>
       <c r="P3"/>
       <c r="Q3">
-        <v>1551.55</v>
+        <v>1451.45</v>
       </c>
       <c r="R3" t="s">
         <v>39</v>
@@ -3373,7 +3376,7 @@
       </c>
       <c r="P4"/>
       <c r="Q4">
-        <v>1451.45</v>
+        <v>1601.6</v>
       </c>
       <c r="R4" t="s">
         <v>39</v>
@@ -3446,7 +3449,7 @@
       </c>
       <c r="P5"/>
       <c r="Q5">
-        <v>1451.45</v>
+        <v>1851.85</v>
       </c>
       <c r="R5" t="s">
         <v>39</v>
@@ -3519,7 +3522,7 @@
       </c>
       <c r="P6"/>
       <c r="Q6">
-        <v>1451.45</v>
+        <v>1851.85</v>
       </c>
       <c r="R6" t="s">
         <v>39</v>
@@ -3592,7 +3595,7 @@
       </c>
       <c r="P7"/>
       <c r="Q7">
-        <v>1451.45</v>
+        <v>1551.55</v>
       </c>
       <c r="R7" t="s">
         <v>39</v>
@@ -3665,7 +3668,7 @@
       </c>
       <c r="P8"/>
       <c r="Q8">
-        <v>1601.6</v>
+        <v>1501.5</v>
       </c>
       <c r="R8" t="s">
         <v>39</v>
@@ -3740,7 +3743,7 @@
       </c>
       <c r="P9"/>
       <c r="Q9">
-        <v>1851.85</v>
+        <v>1451.45</v>
       </c>
       <c r="R9" t="s">
         <v>39</v>
@@ -3813,7 +3816,7 @@
       </c>
       <c r="P10"/>
       <c r="Q10">
-        <v>1851.85</v>
+        <v>1401.4</v>
       </c>
       <c r="R10" t="s">
         <v>39</v>
@@ -3886,7 +3889,7 @@
       </c>
       <c r="P11"/>
       <c r="Q11">
-        <v>1551.55</v>
+        <v>1351.35</v>
       </c>
       <c r="R11" t="s">
         <v>39</v>
@@ -3959,7 +3962,7 @@
       </c>
       <c r="P12"/>
       <c r="Q12">
-        <v>1501.5</v>
+        <v>1351.35</v>
       </c>
       <c r="R12" t="s">
         <v>39</v>
@@ -4032,7 +4035,7 @@
       </c>
       <c r="P13"/>
       <c r="Q13">
-        <v>1451.45</v>
+        <v>1851.85</v>
       </c>
       <c r="R13" t="s">
         <v>39</v>
@@ -4105,7 +4108,7 @@
       </c>
       <c r="P14"/>
       <c r="Q14">
-        <v>1401.4</v>
+        <v>1701.7</v>
       </c>
       <c r="R14" t="s">
         <v>39</v>
@@ -4178,7 +4181,7 @@
       </c>
       <c r="P15"/>
       <c r="Q15">
-        <v>1351.35</v>
+        <v>1451.45</v>
       </c>
       <c r="R15" t="s">
         <v>39</v>
@@ -4251,7 +4254,7 @@
       </c>
       <c r="P16"/>
       <c r="Q16">
-        <v>1351.35</v>
+        <v>1451.45</v>
       </c>
       <c r="R16" t="s">
         <v>39</v>
@@ -4324,7 +4327,7 @@
       </c>
       <c r="P17"/>
       <c r="Q17">
-        <v>1851.85</v>
+        <v>1451.45</v>
       </c>
       <c r="R17" t="s">
         <v>39</v>
@@ -4397,7 +4400,7 @@
       </c>
       <c r="P18"/>
       <c r="Q18">
-        <v>1851.85</v>
+        <v>1451.45</v>
       </c>
       <c r="R18" t="s">
         <v>39</v>
@@ -4470,7 +4473,7 @@
       </c>
       <c r="P19"/>
       <c r="Q19">
-        <v>1451.45</v>
+        <v>1351.35</v>
       </c>
       <c r="R19" t="s">
         <v>39</v>
@@ -4543,7 +4546,7 @@
       </c>
       <c r="P20"/>
       <c r="Q20">
-        <v>1451.45</v>
+        <v>1351.35</v>
       </c>
       <c r="R20" t="s">
         <v>39</v>
@@ -4616,7 +4619,7 @@
       </c>
       <c r="P21"/>
       <c r="Q21">
-        <v>1451.45</v>
+        <v>1351.35</v>
       </c>
       <c r="R21" t="s">
         <v>39</v>
@@ -4689,7 +4692,7 @@
       </c>
       <c r="P22"/>
       <c r="Q22">
-        <v>1451.45</v>
+        <v>1351.35</v>
       </c>
       <c r="R22" t="s">
         <v>39</v>
@@ -5054,7 +5057,7 @@
       </c>
       <c r="P27"/>
       <c r="Q27">
-        <v>1351.35</v>
+        <v>1701.7</v>
       </c>
       <c r="R27" t="s">
         <v>39</v>
@@ -5127,7 +5130,7 @@
       </c>
       <c r="P28"/>
       <c r="Q28">
-        <v>1351.35</v>
+        <v>1701.7</v>
       </c>
       <c r="R28" t="s">
         <v>39</v>
@@ -5200,7 +5203,7 @@
       </c>
       <c r="P29"/>
       <c r="Q29">
-        <v>1351.35</v>
+        <v>1601.6</v>
       </c>
       <c r="R29" t="s">
         <v>39</v>
@@ -5275,7 +5278,7 @@
       </c>
       <c r="P30"/>
       <c r="Q30">
-        <v>1351.35</v>
+        <v>1551.55</v>
       </c>
       <c r="R30" t="s">
         <v>39</v>
@@ -5350,7 +5353,7 @@
       </c>
       <c r="P31"/>
       <c r="Q31">
-        <v>1351.35</v>
+        <v>1451.45</v>
       </c>
       <c r="R31" t="s">
         <v>39</v>
@@ -5423,7 +5426,7 @@
       </c>
       <c r="P32"/>
       <c r="Q32">
-        <v>1351.35</v>
+        <v>1701.7</v>
       </c>
       <c r="R32" t="s">
         <v>39</v>
@@ -5498,7 +5501,7 @@
       </c>
       <c r="P33"/>
       <c r="Q33">
-        <v>1351.35</v>
+        <v>1701.7</v>
       </c>
       <c r="R33" t="s">
         <v>39</v>
@@ -5573,7 +5576,7 @@
       </c>
       <c r="P34"/>
       <c r="Q34">
-        <v>1351.35</v>
+        <v>1701.7</v>
       </c>
       <c r="R34" t="s">
         <v>39</v>
@@ -5646,7 +5649,7 @@
       </c>
       <c r="P35"/>
       <c r="Q35">
-        <v>1351.35</v>
+        <v>1401.4</v>
       </c>
       <c r="R35" t="s">
         <v>39</v>
@@ -5719,7 +5722,7 @@
       </c>
       <c r="P36"/>
       <c r="Q36">
-        <v>1351.35</v>
+        <v>1401.4</v>
       </c>
       <c r="R36" t="s">
         <v>39</v>
@@ -5792,7 +5795,7 @@
       </c>
       <c r="P37"/>
       <c r="Q37">
-        <v>1351.35</v>
+        <v>1401.4</v>
       </c>
       <c r="R37" t="s">
         <v>39</v>
@@ -5865,7 +5868,7 @@
       </c>
       <c r="P38"/>
       <c r="Q38">
-        <v>1351.35</v>
+        <v>1501.5</v>
       </c>
       <c r="R38" t="s">
         <v>39</v>
@@ -5938,7 +5941,7 @@
       </c>
       <c r="P39"/>
       <c r="Q39">
-        <v>1351.35</v>
+        <v>1501.5</v>
       </c>
       <c r="R39" t="s">
         <v>39</v>
@@ -6011,7 +6014,7 @@
       </c>
       <c r="P40"/>
       <c r="Q40">
-        <v>1351.35</v>
+        <v>1501.5</v>
       </c>
       <c r="R40" t="s">
         <v>39</v>
@@ -6084,7 +6087,7 @@
       </c>
       <c r="P41"/>
       <c r="Q41">
-        <v>1351.35</v>
+        <v>1501.5</v>
       </c>
       <c r="R41" t="s">
         <v>39</v>
@@ -6157,7 +6160,7 @@
       </c>
       <c r="P42"/>
       <c r="Q42">
-        <v>1351.35</v>
+        <v>1501.5</v>
       </c>
       <c r="R42" t="s">
         <v>39</v>
@@ -6230,7 +6233,7 @@
       </c>
       <c r="P43"/>
       <c r="Q43">
-        <v>1351.35</v>
+        <v>1501.5</v>
       </c>
       <c r="R43" t="s">
         <v>39</v>
@@ -6303,7 +6306,7 @@
       </c>
       <c r="P44"/>
       <c r="Q44">
-        <v>1351.35</v>
+        <v>1501.5</v>
       </c>
       <c r="R44" t="s">
         <v>39</v>
@@ -6376,7 +6379,7 @@
       </c>
       <c r="P45"/>
       <c r="Q45">
-        <v>1351.35</v>
+        <v>1501.5</v>
       </c>
       <c r="R45" t="s">
         <v>39</v>
@@ -6449,7 +6452,7 @@
       </c>
       <c r="P46"/>
       <c r="Q46">
-        <v>1351.35</v>
+        <v>1501.5</v>
       </c>
       <c r="R46" t="s">
         <v>39</v>
@@ -6522,7 +6525,7 @@
       </c>
       <c r="P47"/>
       <c r="Q47">
-        <v>1351.35</v>
+        <v>1501.5</v>
       </c>
       <c r="R47" t="s">
         <v>39</v>
@@ -6595,7 +6598,7 @@
       </c>
       <c r="P48"/>
       <c r="Q48">
-        <v>1351.35</v>
+        <v>1501.5</v>
       </c>
       <c r="R48" t="s">
         <v>39</v>
@@ -6668,7 +6671,7 @@
       </c>
       <c r="P49"/>
       <c r="Q49">
-        <v>1351.35</v>
+        <v>1501.5</v>
       </c>
       <c r="R49" t="s">
         <v>39</v>
@@ -6741,7 +6744,7 @@
       </c>
       <c r="P50"/>
       <c r="Q50">
-        <v>1351.35</v>
+        <v>1501.5</v>
       </c>
       <c r="R50" t="s">
         <v>39</v>
@@ -6814,7 +6817,7 @@
       </c>
       <c r="P51"/>
       <c r="Q51">
-        <v>1701.7</v>
+        <v>1501.5</v>
       </c>
       <c r="R51" t="s">
         <v>39</v>
@@ -6887,7 +6890,7 @@
       </c>
       <c r="P52"/>
       <c r="Q52">
-        <v>1601.6</v>
+        <v>1501.5</v>
       </c>
       <c r="R52" t="s">
         <v>39</v>
@@ -6960,7 +6963,7 @@
       </c>
       <c r="P53"/>
       <c r="Q53">
-        <v>1701.7</v>
+        <v>1501.5</v>
       </c>
       <c r="R53" t="s">
         <v>39</v>
@@ -7033,7 +7036,7 @@
       </c>
       <c r="P54"/>
       <c r="Q54">
-        <v>1551.55</v>
+        <v>1501.5</v>
       </c>
       <c r="R54" t="s">
         <v>39</v>
@@ -7106,7 +7109,7 @@
       </c>
       <c r="P55"/>
       <c r="Q55">
-        <v>1351.35</v>
+        <v>1501.5</v>
       </c>
       <c r="R55" t="s">
         <v>39</v>
@@ -7179,7 +7182,7 @@
       </c>
       <c r="P56"/>
       <c r="Q56">
-        <v>1351.35</v>
+        <v>1501.5</v>
       </c>
       <c r="R56" t="s">
         <v>39</v>
@@ -7252,7 +7255,7 @@
       </c>
       <c r="P57"/>
       <c r="Q57">
-        <v>1451.45</v>
+        <v>1501.5</v>
       </c>
       <c r="R57" t="s">
         <v>39</v>
@@ -7325,7 +7328,7 @@
       </c>
       <c r="P58"/>
       <c r="Q58">
-        <v>1701.7</v>
+        <v>1501.5</v>
       </c>
       <c r="R58" t="s">
         <v>39</v>
@@ -7400,7 +7403,7 @@
       </c>
       <c r="P59"/>
       <c r="Q59">
-        <v>1701.7</v>
+        <v>1451.45</v>
       </c>
       <c r="R59" t="s">
         <v>39</v>
@@ -7475,7 +7478,7 @@
       </c>
       <c r="P60"/>
       <c r="Q60">
-        <v>1701.7</v>
+        <v>1451.45</v>
       </c>
       <c r="R60" t="s">
         <v>39</v>
@@ -7550,7 +7553,7 @@
       </c>
       <c r="P61"/>
       <c r="Q61">
-        <v>1401.4</v>
+        <v>1451.45</v>
       </c>
       <c r="R61" t="s">
         <v>39</v>
@@ -7625,7 +7628,7 @@
       </c>
       <c r="P62"/>
       <c r="Q62">
-        <v>1401.4</v>
+        <v>1451.45</v>
       </c>
       <c r="R62" t="s">
         <v>39</v>
@@ -7700,7 +7703,7 @@
       </c>
       <c r="P63"/>
       <c r="Q63">
-        <v>1401.4</v>
+        <v>1451.45</v>
       </c>
       <c r="R63" t="s">
         <v>39</v>
@@ -7775,7 +7778,7 @@
       </c>
       <c r="P64"/>
       <c r="Q64">
-        <v>1501.5</v>
+        <v>1451.45</v>
       </c>
       <c r="R64" t="s">
         <v>39</v>
@@ -7850,7 +7853,7 @@
       </c>
       <c r="P65"/>
       <c r="Q65">
-        <v>1501.5</v>
+        <v>1451.45</v>
       </c>
       <c r="R65" t="s">
         <v>39</v>
@@ -7925,7 +7928,7 @@
       </c>
       <c r="P66"/>
       <c r="Q66">
-        <v>1501.5</v>
+        <v>1451.45</v>
       </c>
       <c r="R66" t="s">
         <v>39</v>
@@ -8000,7 +8003,7 @@
       </c>
       <c r="P67"/>
       <c r="Q67">
-        <v>1501.5</v>
+        <v>1451.45</v>
       </c>
       <c r="R67" t="s">
         <v>39</v>
@@ -8075,7 +8078,7 @@
       </c>
       <c r="P68"/>
       <c r="Q68">
-        <v>1501.5</v>
+        <v>1451.45</v>
       </c>
       <c r="R68" t="s">
         <v>39</v>
@@ -8150,7 +8153,7 @@
       </c>
       <c r="P69"/>
       <c r="Q69">
-        <v>1501.5</v>
+        <v>1451.45</v>
       </c>
       <c r="R69" t="s">
         <v>39</v>
@@ -8225,7 +8228,7 @@
       </c>
       <c r="P70"/>
       <c r="Q70">
-        <v>1501.5</v>
+        <v>1451.45</v>
       </c>
       <c r="R70" t="s">
         <v>39</v>
@@ -8300,7 +8303,7 @@
       </c>
       <c r="P71"/>
       <c r="Q71">
-        <v>1501.5</v>
+        <v>1451.45</v>
       </c>
       <c r="R71" t="s">
         <v>39</v>
@@ -8375,7 +8378,7 @@
       </c>
       <c r="P72"/>
       <c r="Q72">
-        <v>1501.5</v>
+        <v>1451.45</v>
       </c>
       <c r="R72" t="s">
         <v>39</v>
@@ -8450,7 +8453,7 @@
       </c>
       <c r="P73"/>
       <c r="Q73">
-        <v>1501.5</v>
+        <v>1451.45</v>
       </c>
       <c r="R73" t="s">
         <v>39</v>
@@ -8525,7 +8528,7 @@
       </c>
       <c r="P74"/>
       <c r="Q74">
-        <v>1501.5</v>
+        <v>1451.45</v>
       </c>
       <c r="R74" t="s">
         <v>39</v>
@@ -8598,7 +8601,7 @@
       </c>
       <c r="P75"/>
       <c r="Q75">
-        <v>1501.5</v>
+        <v>1801.8</v>
       </c>
       <c r="R75" t="s">
         <v>39</v>
@@ -8671,7 +8674,7 @@
       </c>
       <c r="P76"/>
       <c r="Q76">
-        <v>1501.5</v>
+        <v>1551.55</v>
       </c>
       <c r="R76" t="s">
         <v>39</v>
@@ -8746,7 +8749,7 @@
       </c>
       <c r="P77"/>
       <c r="Q77">
-        <v>1501.5</v>
+        <v>1601.6</v>
       </c>
       <c r="R77" t="s">
         <v>39</v>
@@ -8819,7 +8822,7 @@
       </c>
       <c r="P78"/>
       <c r="Q78">
-        <v>1501.5</v>
+        <v>1351.35</v>
       </c>
       <c r="R78" t="s">
         <v>39</v>
@@ -8892,7 +8895,7 @@
       </c>
       <c r="P79"/>
       <c r="Q79">
-        <v>1501.5</v>
+        <v>1351.35</v>
       </c>
       <c r="R79" t="s">
         <v>39</v>
@@ -8965,7 +8968,7 @@
       </c>
       <c r="P80"/>
       <c r="Q80">
-        <v>1501.5</v>
+        <v>1351.35</v>
       </c>
       <c r="R80" t="s">
         <v>39</v>
@@ -9038,7 +9041,7 @@
       </c>
       <c r="P81"/>
       <c r="Q81">
-        <v>1501.5</v>
+        <v>1351.35</v>
       </c>
       <c r="R81" t="s">
         <v>39</v>
@@ -9113,7 +9116,7 @@
         <v>524</v>
       </c>
       <c r="Q82">
-        <v>1451.45</v>
+        <v>1351.35</v>
       </c>
       <c r="R82" t="s">
         <v>39</v>
@@ -9188,7 +9191,7 @@
         <v>524</v>
       </c>
       <c r="Q83">
-        <v>1451.45</v>
+        <v>1351.35</v>
       </c>
       <c r="R83" t="s">
         <v>39</v>
@@ -9261,7 +9264,7 @@
       </c>
       <c r="P84"/>
       <c r="Q84">
-        <v>1851.85</v>
+        <v>1451.45</v>
       </c>
       <c r="R84" t="s">
         <v>39</v>
@@ -9334,7 +9337,7 @@
       </c>
       <c r="P85"/>
       <c r="Q85">
-        <v>1851.85</v>
+        <v>1451.45</v>
       </c>
       <c r="R85" t="s">
         <v>39</v>
@@ -9409,7 +9412,7 @@
         <v>524</v>
       </c>
       <c r="Q86">
-        <v>1501.5</v>
+        <v>1451.45</v>
       </c>
       <c r="R86" t="s">
         <v>39</v>
@@ -9484,7 +9487,7 @@
         <v>524</v>
       </c>
       <c r="Q87">
-        <v>1501.5</v>
+        <v>1451.45</v>
       </c>
       <c r="R87" t="s">
         <v>39</v>
@@ -9559,7 +9562,7 @@
         <v>524</v>
       </c>
       <c r="Q88">
-        <v>1501.5</v>
+        <v>1451.45</v>
       </c>
       <c r="R88" t="s">
         <v>39</v>
@@ -9634,7 +9637,7 @@
         <v>524</v>
       </c>
       <c r="Q89">
-        <v>1501.5</v>
+        <v>1351.35</v>
       </c>
       <c r="R89" t="s">
         <v>39</v>
@@ -9709,7 +9712,7 @@
         <v>524</v>
       </c>
       <c r="Q90">
-        <v>1501.5</v>
+        <v>1351.35</v>
       </c>
       <c r="R90" t="s">
         <v>39</v>
@@ -9784,7 +9787,7 @@
         <v>524</v>
       </c>
       <c r="Q91">
-        <v>1501.5</v>
+        <v>1351.35</v>
       </c>
       <c r="R91" t="s">
         <v>39</v>
@@ -9859,7 +9862,7 @@
         <v>524</v>
       </c>
       <c r="Q92">
-        <v>1451.45</v>
+        <v>1351.35</v>
       </c>
       <c r="R92" t="s">
         <v>39</v>
@@ -9934,7 +9937,7 @@
         <v>524</v>
       </c>
       <c r="Q93">
-        <v>1451.45</v>
+        <v>1351.35</v>
       </c>
       <c r="R93" t="s">
         <v>39</v>
@@ -10007,7 +10010,7 @@
       </c>
       <c r="P94"/>
       <c r="Q94">
-        <v>1351.35</v>
+        <v>1501.5</v>
       </c>
       <c r="R94" t="s">
         <v>39</v>
@@ -10082,7 +10085,7 @@
         <v>524</v>
       </c>
       <c r="Q95">
-        <v>1451.45</v>
+        <v>1501.5</v>
       </c>
       <c r="R95" t="s">
         <v>39</v>
@@ -10157,7 +10160,7 @@
         <v>524</v>
       </c>
       <c r="Q96">
-        <v>1451.45</v>
+        <v>1501.5</v>
       </c>
       <c r="R96" t="s">
         <v>39</v>
@@ -10305,7 +10308,7 @@
       </c>
       <c r="P98"/>
       <c r="Q98">
-        <v>1701.7</v>
+        <v>1351.35</v>
       </c>
       <c r="R98" t="s">
         <v>39</v>
@@ -10378,7 +10381,7 @@
       </c>
       <c r="P99"/>
       <c r="Q99">
-        <v>1451.45</v>
+        <v>1351.35</v>
       </c>
       <c r="R99" t="s">
         <v>39</v>
@@ -10526,7 +10529,7 @@
         <v>524</v>
       </c>
       <c r="Q101">
-        <v>1451.45</v>
+        <v>1351.35</v>
       </c>
       <c r="R101" t="s">
         <v>39</v>
@@ -10599,7 +10602,7 @@
       </c>
       <c r="P102"/>
       <c r="Q102">
-        <v>1451.45</v>
+        <v>1351.35</v>
       </c>
       <c r="R102" t="s">
         <v>39</v>
@@ -10674,7 +10677,7 @@
         <v>524</v>
       </c>
       <c r="Q103">
-        <v>1501.5</v>
+        <v>1651.65</v>
       </c>
       <c r="R103" t="s">
         <v>39</v>
@@ -10751,7 +10754,7 @@
         <v>646</v>
       </c>
       <c r="Q104">
-        <v>1351.35</v>
+        <v>1451.45</v>
       </c>
       <c r="R104" t="s">
         <v>39</v>
@@ -10826,7 +10829,7 @@
       </c>
       <c r="P105"/>
       <c r="Q105">
-        <v>1501.5</v>
+        <v>1451.45</v>
       </c>
       <c r="R105" t="s">
         <v>39</v>
@@ -10899,7 +10902,7 @@
       </c>
       <c r="P106"/>
       <c r="Q106">
-        <v>1501.5</v>
+        <v>1851.85</v>
       </c>
       <c r="R106" t="s">
         <v>39</v>
@@ -10972,7 +10975,7 @@
       </c>
       <c r="P107"/>
       <c r="Q107">
-        <v>1501.5</v>
+        <v>1851.85</v>
       </c>
       <c r="R107" t="s">
         <v>39</v>
@@ -11045,7 +11048,7 @@
       </c>
       <c r="P108"/>
       <c r="Q108">
-        <v>1501.5</v>
+        <v>1851.85</v>
       </c>
       <c r="R108" t="s">
         <v>39</v>
@@ -11120,7 +11123,7 @@
         <v>524</v>
       </c>
       <c r="Q109">
-        <v>1501.5</v>
+        <v>1351.35</v>
       </c>
       <c r="R109" t="s">
         <v>39</v>
@@ -11193,7 +11196,7 @@
       </c>
       <c r="P110"/>
       <c r="Q110">
-        <v>1451.45</v>
+        <v>1351.35</v>
       </c>
       <c r="R110" t="s">
         <v>39</v>
@@ -11268,7 +11271,7 @@
         <v>524</v>
       </c>
       <c r="Q111">
-        <v>1451.45</v>
+        <v>1351.35</v>
       </c>
       <c r="R111" t="s">
         <v>39</v>
@@ -11341,7 +11344,7 @@
       </c>
       <c r="P112"/>
       <c r="Q112">
-        <v>1451.45</v>
+        <v>1351.35</v>
       </c>
       <c r="R112" t="s">
         <v>39</v>
@@ -11416,7 +11419,7 @@
         <v>524</v>
       </c>
       <c r="Q113">
-        <v>1451.45</v>
+        <v>1351.35</v>
       </c>
       <c r="R113" t="s">
         <v>39</v>
@@ -11491,7 +11494,7 @@
         <v>524</v>
       </c>
       <c r="Q114">
-        <v>1451.45</v>
+        <v>1351.35</v>
       </c>
       <c r="R114" t="s">
         <v>39</v>
@@ -11566,7 +11569,7 @@
         <v>524</v>
       </c>
       <c r="Q115">
-        <v>1451.45</v>
+        <v>1351.35</v>
       </c>
       <c r="R115" t="s">
         <v>39</v>
@@ -11639,7 +11642,7 @@
       </c>
       <c r="P116"/>
       <c r="Q116">
-        <v>1451.45</v>
+        <v>1351.35</v>
       </c>
       <c r="R116" t="s">
         <v>39</v>
@@ -11787,7 +11790,7 @@
         <v>524</v>
       </c>
       <c r="Q118">
-        <v>1451.45</v>
+        <v>1351.35</v>
       </c>
       <c r="R118" t="s">
         <v>39</v>
@@ -11862,7 +11865,7 @@
         <v>524</v>
       </c>
       <c r="Q119">
-        <v>1451.45</v>
+        <v>1351.35</v>
       </c>
       <c r="R119" t="s">
         <v>39</v>
@@ -11937,7 +11940,7 @@
         <v>524</v>
       </c>
       <c r="Q120">
-        <v>1501.5</v>
+        <v>1451.45</v>
       </c>
       <c r="R120" t="s">
         <v>39</v>
@@ -12012,7 +12015,7 @@
         <v>524</v>
       </c>
       <c r="Q121">
-        <v>1501.5</v>
+        <v>1451.45</v>
       </c>
       <c r="R121" t="s">
         <v>39</v>
@@ -12087,7 +12090,7 @@
         <v>524</v>
       </c>
       <c r="Q122">
-        <v>1501.5</v>
+        <v>1451.45</v>
       </c>
       <c r="R122" t="s">
         <v>39</v>
@@ -12162,7 +12165,7 @@
         <v>524</v>
       </c>
       <c r="Q123">
-        <v>1451.45</v>
+        <v>1351.35</v>
       </c>
       <c r="R123" t="s">
         <v>39</v>
@@ -12237,7 +12240,7 @@
         <v>524</v>
       </c>
       <c r="Q124">
-        <v>1451.45</v>
+        <v>1351.35</v>
       </c>
       <c r="R124" t="s">
         <v>39</v>
@@ -12312,7 +12315,7 @@
         <v>524</v>
       </c>
       <c r="Q125">
-        <v>1451.45</v>
+        <v>1501.5</v>
       </c>
       <c r="R125" t="s">
         <v>39</v>
@@ -12387,7 +12390,7 @@
         <v>524</v>
       </c>
       <c r="Q126">
-        <v>1551.55</v>
+        <v>1501.5</v>
       </c>
       <c r="R126" t="s">
         <v>39</v>
@@ -12462,7 +12465,7 @@
         <v>524</v>
       </c>
       <c r="Q127">
-        <v>1801.8</v>
+        <v>1501.5</v>
       </c>
       <c r="R127" t="s">
         <v>39</v>
@@ -12537,7 +12540,7 @@
         <v>524</v>
       </c>
       <c r="Q128">
-        <v>1451.45</v>
+        <v>1501.5</v>
       </c>
       <c r="R128" t="s">
         <v>39</v>
@@ -12612,7 +12615,7 @@
         <v>524</v>
       </c>
       <c r="Q129">
-        <v>1451.45</v>
+        <v>1501.5</v>
       </c>
       <c r="R129" t="s">
         <v>39</v>
@@ -12687,7 +12690,7 @@
         <v>524</v>
       </c>
       <c r="Q130">
-        <v>1601.6</v>
+        <v>1501.5</v>
       </c>
       <c r="R130" t="s">
         <v>39</v>
@@ -12762,7 +12765,7 @@
         <v>524</v>
       </c>
       <c r="Q131">
-        <v>1351.35</v>
+        <v>1501.5</v>
       </c>
       <c r="R131" t="s">
         <v>39</v>
@@ -12837,7 +12840,7 @@
         <v>524</v>
       </c>
       <c r="Q132">
-        <v>1351.35</v>
+        <v>1501.5</v>
       </c>
       <c r="R132" t="s">
         <v>39</v>
@@ -12912,7 +12915,7 @@
         <v>524</v>
       </c>
       <c r="Q133">
-        <v>1351.35</v>
+        <v>1501.5</v>
       </c>
       <c r="R133" t="s">
         <v>39</v>
@@ -13100,7 +13103,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="X1:X1048576" xr:uid="{B7F49F50-5CB2-4CAA-8452-128DC5ABE3C9}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="X1:X1048576" xr:uid="{B6FA812F-EC7A-487B-AC4F-4DA35FAD9CE7}">
       <formula1>#REF!</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>